<commit_message>
Update Plan de mejora, seguimiento y evaluación de la empleabilidad.xlsx
</commit_message>
<xml_diff>
--- a/Plan de mejoras/Plan de mejora, seguimiento y evaluación de la empleabilidad.xlsx
+++ b/Plan de mejoras/Plan de mejora, seguimiento y evaluación de la empleabilidad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aaven\Documents\GitHub\cdia\Plan de mejoras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAB64529-89B0-4434-A3D0-1DE9EF58ED56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F6F4CEC-B670-430F-A3FB-322C38CD3995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B5333BF1-CD0B-4BEF-BD63-D108514CC92F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Hallazgo</t>
   </si>
@@ -87,10 +87,16 @@
     <t>Mayo a Junio - 2025</t>
   </si>
   <si>
-    <t>Las observaciones obtenidas en la reunión del comité consultivo 2024</t>
-  </si>
-  <si>
     <t>Número de estudiantes que realizan la práctica / Número de estudiantes disponibles para realizar la práctica</t>
+  </si>
+  <si>
+    <t>100%, revisión en el sistema de prácticas</t>
+  </si>
+  <si>
+    <t>Las observaciones obtenidas de la reunión del comité consultivo 2024</t>
+  </si>
+  <si>
+    <t>Ciencia de Datos e Inteligencia Artificial</t>
   </si>
 </sst>
 </file>
@@ -321,6 +327,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -338,9 +347,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -659,7 +665,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -668,26 +674,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="12"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="13"/>
     </row>
     <row r="2" spans="1:7" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="15"/>
+      <c r="B2" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="16"/>
     </row>
     <row r="3" spans="1:7" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
@@ -736,26 +744,26 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="109.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>20</v>
+      <c r="B5" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="10" t="s">
         <v>21</v>
-      </c>
-      <c r="G5" s="16">
-        <v>0.7</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -832,23 +840,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="00202844-26d8-4353-ab03-f656441a0c4d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010036BCD0FF6F54534EBF74DACC859E5FFC" ma:contentTypeVersion="18" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="dd2df6d5db0ef0cd439909e80db364b4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3f5cbb17-365e-4bb8-8637-abb0fdfd4339" xmlns:ns4="00202844-26d8-4353-ab03-f656441a0c4d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="02606619b34f6f37bea63d8d11fc113e" ns3:_="" ns4:_="">
     <xsd:import namespace="3f5cbb17-365e-4bb8-8637-abb0fdfd4339"/>
@@ -1101,32 +1092,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3809A7E7-D686-438D-9548-304F6D63D3D8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="3f5cbb17-365e-4bb8-8637-abb0fdfd4339"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="00202844-26d8-4353-ab03-f656441a0c4d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{393688C4-1BD5-4894-86BC-613BF4B1711B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="00202844-26d8-4353-ab03-f656441a0c4d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67631633-EA2C-49E9-A657-A2184E5D6896}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1143,4 +1126,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{393688C4-1BD5-4894-86BC-613BF4B1711B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3809A7E7-D686-438D-9548-304F6D63D3D8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="3f5cbb17-365e-4bb8-8637-abb0fdfd4339"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="00202844-26d8-4353-ab03-f656441a0c4d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>